<commit_message>
More on graphs and analysis
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Threads</t>
   </si>
@@ -121,12 +122,51 @@
   <si>
     <t>Time (ms)</t>
   </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>Floyd-Warshal</t>
+  </si>
+  <si>
+    <t>Time( Seconds)</t>
+  </si>
+  <si>
+    <t>Threads/Processes</t>
+  </si>
+  <si>
+    <t>3000 Nodes</t>
+  </si>
+  <si>
+    <t>1 (Serial Version)</t>
+  </si>
+  <si>
+    <t>Floyd-Warshal OMP (FW OMP)</t>
+  </si>
+  <si>
+    <t>SqaureSum OMP (SS OMP)</t>
+  </si>
+  <si>
+    <t>SqaureSum MPI (SS MPI)</t>
+  </si>
+  <si>
+    <t>(SS OMP) / (FW OMP)</t>
+  </si>
+  <si>
+    <t>(SS MPI) / (FW OMP)</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Time(S)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,13 +212,68 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADF6FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACF8FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,7 +285,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="481">
+  <cellStyleXfs count="515">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -672,15 +767,85 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="481">
+  <cellStyles count="515">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -921,6 +1086,23 @@
     <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1161,6 +1343,23 @@
     <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1218,7 +1417,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$10:$I$20</c:f>
+              <c:f>Sheet1!$P$43:$P$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1260,7 +1459,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$10:$H$20</c:f>
+              <c:f>Sheet1!$O$43:$O$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1500,11 +1699,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="659296344"/>
-        <c:axId val="659301896"/>
+        <c:axId val="659212408"/>
+        <c:axId val="684513688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="659296344"/>
+        <c:axId val="659212408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,12 +1732,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="659301896"/>
+        <c:crossAx val="684513688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="659301896"/>
+        <c:axId val="684513688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1568,7 +1767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="659296344"/>
+        <c:crossAx val="659212408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1577,6 +1776,1112 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>OMP 2 Threads</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$R$10:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$Q$10:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>109492.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600252.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>1.63254E6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>3.71435E6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>7.16933E6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.37744E7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2.41049E7</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2.87276E7</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>4.14226E7</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5.13324E7</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>7.91247E7</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>9.28684E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="723835112"/>
+        <c:axId val="659424408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="723835112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="659424408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="659424408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Micro Seconds (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="723835112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Floyd-Warshal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> OMP vs Serial</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Serial</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$O$10:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$L$10:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.17E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.06E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.283E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.653E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.141E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.511E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.733E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4482E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6452E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>7 Threads</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$O$10:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$N$10:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50003.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206030.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>522900.0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.1872E6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2.54454E6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>4.72506E6</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>8.25255E6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1.13538E7</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>1.59946E7</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>2.15132E7</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>2.82679E7</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>3.64578E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2 Threads</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$O$10:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1900.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3400.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$Q$10:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>109492.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600252.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>1.63254E6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>3.71435E6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>7.16933E6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.37744E7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2.41049E7</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2.87276E7</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>4.14226E7</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5.13324E7</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>7.91247E7</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>9.28684E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="672732968"/>
+        <c:axId val="730578952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="672732968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> of Nodes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="730578952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="730578952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Spent on Computation (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="672732968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.202532320087896"/>
+          <c:y val="0.14370546147485"/>
+          <c:w val="0.132351400842337"/>
+          <c:h val="0.162086793945277"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>up Plot (3000 Nodes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(SS OMP) / (FW OMP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet4!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$E$6:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>15.73028100389572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.27099825945806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.91231469002695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.88163000317062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.2203164064101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.07311489483474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.06230149655716</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.35905924015551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.10034865346187</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.75592154350053</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.378933879629396</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(SS MPI) / (FW OMP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet4!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$F$6:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>15.5337094966539</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.21203224916698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.77177392183289</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.50096880205738</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.30062707488012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.03575005621078</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.71199532484691</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.517571884984025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.29310301581064</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.048409329460811</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.372425537654805</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="728955272"/>
+        <c:axId val="682898296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="728955272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t># of Threads/Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="682898296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="682898296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="728955272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.690151468496605"/>
+          <c:y val="0.166815617767129"/>
+          <c:w val="0.22703220770873"/>
+          <c:h val="0.112352528650942"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1951,11 +3256,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="659349736"/>
-        <c:axId val="659355176"/>
+        <c:axId val="677175992"/>
+        <c:axId val="639330728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="659349736"/>
+        <c:axId val="677175992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,12 +3289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="659355176"/>
+        <c:crossAx val="639330728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="659355176"/>
+        <c:axId val="639330728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +3329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="659349736"/>
+        <c:crossAx val="677175992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2047,6 +3352,477 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Parallelized</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Floyd-Warshal vs SqaureSum (3000 Nodes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SquareSum OMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$P$59:$P$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$43:$O$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>731.252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>576.302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>449.054</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>593.745</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>550.838</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>510.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>434.153</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>424.992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>385.13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>373.773</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>151.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Floyd-Warshal OMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$P$59:$P$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$59:$O$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>46.4869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.5419</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.8699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.5192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.5692</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.6785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.979</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.9206</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.7227</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.7234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>SquareSum MPI</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$P$59:$P$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$57:$R$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>722.114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>605.984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>588.181</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>447.092</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>396.252</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>235.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>328.867</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>195.299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>198.376</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190.93</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>174.899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="724285448"/>
+        <c:axId val="670455992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="724285448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> of Threads/Processes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="670455992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="670455992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> Spent on Computation (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="724285448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.724786962202412"/>
+          <c:y val="0.124932323544393"/>
+          <c:w val="0.23735775318834"/>
+          <c:h val="0.173890331577058"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2509,11 +4285,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="825583096"/>
-        <c:axId val="825588760"/>
+        <c:axId val="535563832"/>
+        <c:axId val="676610728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="825583096"/>
+        <c:axId val="535563832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14.0"/>
@@ -2544,12 +4320,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="825588760"/>
+        <c:crossAx val="676610728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="825588760"/>
+        <c:axId val="676610728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -2580,7 +4356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="825583096"/>
+        <c:crossAx val="535563832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2602,7 +4378,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2956,11 +4732,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="825633816"/>
-        <c:axId val="825639560"/>
+        <c:axId val="723654120"/>
+        <c:axId val="624706952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="825633816"/>
+        <c:axId val="723654120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2994,12 +4770,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="825639560"/>
+        <c:crossAx val="624706952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="825639560"/>
+        <c:axId val="624706952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3029,7 +4805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="825633816"/>
+        <c:crossAx val="723654120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3051,7 +4827,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3158,11 +4934,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="723110024"/>
-        <c:axId val="723117240"/>
+        <c:axId val="659522584"/>
+        <c:axId val="723772136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="723110024"/>
+        <c:axId val="659522584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3195,7 +4971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="723117240"/>
+        <c:crossAx val="723772136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3203,7 +4979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="723117240"/>
+        <c:axId val="723772136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3238,7 +5014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="723110024"/>
+        <c:crossAx val="659522584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3255,7 +5031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3362,11 +5138,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="730660792"/>
-        <c:axId val="730293048"/>
+        <c:axId val="677097848"/>
+        <c:axId val="676384168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="730660792"/>
+        <c:axId val="677097848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3394,7 +5170,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="730293048"/>
+        <c:crossAx val="676384168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3402,7 +5178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="730293048"/>
+        <c:axId val="676384168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3437,7 +5213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="730660792"/>
+        <c:crossAx val="677097848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3454,7 +5230,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3556,11 +5332,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="729013736"/>
-        <c:axId val="672441096"/>
+        <c:axId val="724040952"/>
+        <c:axId val="624586952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="729013736"/>
+        <c:axId val="724040952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3593,7 +5369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672441096"/>
+        <c:crossAx val="624586952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3601,7 +5377,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="672441096"/>
+        <c:axId val="624586952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3636,7 +5412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729013736"/>
+        <c:crossAx val="724040952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3653,7 +5429,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3800,11 +5576,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="677203144"/>
-        <c:axId val="676576584"/>
+        <c:axId val="676933608"/>
+        <c:axId val="676942920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="677203144"/>
+        <c:axId val="676933608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3833,7 +5609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="676576584"/>
+        <c:crossAx val="676942920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3841,7 +5617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="676576584"/>
+        <c:axId val="676942920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3871,7 +5647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="677203144"/>
+        <c:crossAx val="676933608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3881,241 +5657,6 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>OMP 2 Threads</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$R$10:$R$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>400.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1300.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1600.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1900.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2200.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2800.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3100.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3400.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3700.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$Q$10:$Q$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>109492.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>600252.0</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>1.63254E6</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>3.71435E6</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>7.16933E6</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1.37744E7</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2.41049E7</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>2.87276E7</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>4.14226E7</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>5.13324E7</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>7.91247E7</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>9.28684E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="673206584"/>
-        <c:axId val="728980136"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="673206584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># of Nodes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="728980136"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="728980136"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time in Micro Seconds (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="673206584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4185,6 +5726,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4263,15 +5834,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4293,15 +5864,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4323,15 +5894,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4382,16 +5953,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4405,6 +5976,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4735,18 +6371,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:AD101"/>
+  <dimension ref="B7:AD101"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView showRuler="0" topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39:S70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="7" spans="2:21">
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="8" spans="2:21">
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -4754,9 +6396,6 @@
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="N8" s="2" t="s">
         <v>5</v>
       </c>
@@ -4780,12 +6419,6 @@
       <c r="F9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
       <c r="N9" t="s">
         <v>1</v>
       </c>
@@ -4818,12 +6451,6 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>731.25199999999995</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
       <c r="N10">
         <v>1.7882800000000001</v>
       </c>
@@ -4856,12 +6483,6 @@
       <c r="F11">
         <v>2</v>
       </c>
-      <c r="H11">
-        <v>576.30200000000002</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
       <c r="N11">
         <v>2.8241100000000001</v>
       </c>
@@ -4894,12 +6515,6 @@
       <c r="F12">
         <v>3</v>
       </c>
-      <c r="H12">
-        <v>449.05399999999997</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
       <c r="N12">
         <v>15.5481</v>
       </c>
@@ -4932,12 +6547,6 @@
       <c r="F13">
         <v>4</v>
       </c>
-      <c r="H13">
-        <v>593.745</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
       <c r="N13">
         <v>22.900700000000001</v>
       </c>
@@ -4970,12 +6579,6 @@
       <c r="F14">
         <v>5</v>
       </c>
-      <c r="H14">
-        <v>550.83799999999997</v>
-      </c>
-      <c r="I14">
-        <v>6</v>
-      </c>
       <c r="N14">
         <v>46.275599999999997</v>
       </c>
@@ -5008,12 +6611,6 @@
       <c r="F15">
         <v>6</v>
       </c>
-      <c r="H15">
-        <v>510.23</v>
-      </c>
-      <c r="I15">
-        <v>7</v>
-      </c>
       <c r="N15">
         <v>72.423299999999998</v>
       </c>
@@ -5046,12 +6643,6 @@
       <c r="F16">
         <v>7</v>
       </c>
-      <c r="H16">
-        <v>434.15300000000002</v>
-      </c>
-      <c r="I16">
-        <v>8</v>
-      </c>
       <c r="N16">
         <v>120.127</v>
       </c>
@@ -5084,12 +6675,6 @@
       <c r="F17">
         <v>8</v>
       </c>
-      <c r="H17">
-        <v>424.99200000000002</v>
-      </c>
-      <c r="I17">
-        <v>9</v>
-      </c>
       <c r="N17">
         <v>95.634500000000003</v>
       </c>
@@ -5122,12 +6707,6 @@
       <c r="F18">
         <v>9</v>
       </c>
-      <c r="H18">
-        <v>385.13</v>
-      </c>
-      <c r="I18">
-        <v>10</v>
-      </c>
       <c r="N18">
         <v>150.37799999999999</v>
       </c>
@@ -5154,12 +6733,6 @@
       <c r="F19">
         <v>10</v>
       </c>
-      <c r="H19">
-        <v>373.77300000000002</v>
-      </c>
-      <c r="I19">
-        <v>11</v>
-      </c>
       <c r="N19">
         <v>207.447</v>
       </c>
@@ -5186,12 +6759,6 @@
       <c r="F20">
         <v>12</v>
       </c>
-      <c r="H20">
-        <v>151.33000000000001</v>
-      </c>
-      <c r="I20">
-        <v>12</v>
-      </c>
       <c r="N20">
         <v>293.65600000000001</v>
       </c>
@@ -5231,6 +6798,11 @@
         <v>3700</v>
       </c>
     </row>
+    <row r="39" spans="3:26">
+      <c r="O39" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="40" spans="3:26">
       <c r="C40" s="2" t="s">
         <v>9</v>
@@ -5238,6 +6810,9 @@
       <c r="I40" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="O40" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="R40" s="3" t="s">
         <v>11</v>
       </c>
@@ -5259,6 +6834,12 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
+      <c r="O41" t="s">
+        <v>1</v>
+      </c>
+      <c r="P41" t="s">
+        <v>0</v>
+      </c>
       <c r="R41" t="s">
         <v>1</v>
       </c>
@@ -5311,6 +6892,12 @@
       <c r="J43">
         <v>3</v>
       </c>
+      <c r="O43">
+        <v>731.25199999999995</v>
+      </c>
+      <c r="P43">
+        <v>2</v>
+      </c>
       <c r="R43">
         <v>600.11599999999999</v>
       </c>
@@ -5337,6 +6924,12 @@
       <c r="J44">
         <v>4</v>
       </c>
+      <c r="O44">
+        <v>576.30200000000002</v>
+      </c>
+      <c r="P44">
+        <v>3</v>
+      </c>
       <c r="R44">
         <v>550.18200000000002</v>
       </c>
@@ -5363,6 +6956,12 @@
       <c r="J45">
         <v>5</v>
       </c>
+      <c r="O45">
+        <v>449.05399999999997</v>
+      </c>
+      <c r="P45">
+        <v>4</v>
+      </c>
       <c r="R45">
         <v>814.97900000000004</v>
       </c>
@@ -5389,6 +6988,12 @@
       <c r="J46">
         <v>6</v>
       </c>
+      <c r="O46">
+        <v>593.745</v>
+      </c>
+      <c r="P46">
+        <v>5</v>
+      </c>
       <c r="R46">
         <v>798.77</v>
       </c>
@@ -5415,6 +7020,12 @@
       <c r="J47">
         <v>7</v>
       </c>
+      <c r="O47">
+        <v>550.83799999999997</v>
+      </c>
+      <c r="P47">
+        <v>6</v>
+      </c>
       <c r="R47">
         <v>804.846</v>
       </c>
@@ -5441,6 +7052,12 @@
       <c r="J48">
         <v>8</v>
       </c>
+      <c r="O48">
+        <v>510.23</v>
+      </c>
+      <c r="P48">
+        <v>7</v>
+      </c>
       <c r="R48">
         <v>743.67200000000003</v>
       </c>
@@ -5467,6 +7084,12 @@
       <c r="J49">
         <v>9</v>
       </c>
+      <c r="O49">
+        <v>434.15300000000002</v>
+      </c>
+      <c r="P49">
+        <v>8</v>
+      </c>
       <c r="R49">
         <v>591.63699999999994</v>
       </c>
@@ -5494,6 +7117,12 @@
       <c r="J50">
         <v>10</v>
       </c>
+      <c r="O50">
+        <v>424.99200000000002</v>
+      </c>
+      <c r="P50">
+        <v>9</v>
+      </c>
       <c r="R50">
         <v>590.73199999999997</v>
       </c>
@@ -5514,6 +7143,12 @@
       <c r="J51">
         <v>11</v>
       </c>
+      <c r="O51">
+        <v>385.13</v>
+      </c>
+      <c r="P51">
+        <v>10</v>
+      </c>
       <c r="R51">
         <v>587.37</v>
       </c>
@@ -5534,6 +7169,12 @@
       <c r="J52">
         <v>12</v>
       </c>
+      <c r="O52">
+        <v>373.77300000000002</v>
+      </c>
+      <c r="P52">
+        <v>11</v>
+      </c>
       <c r="R52">
         <v>193.601</v>
       </c>
@@ -5549,6 +7190,12 @@
       <c r="AC52" s="1"/>
     </row>
     <row r="53" spans="3:30">
+      <c r="O53">
+        <v>151.33000000000001</v>
+      </c>
+      <c r="P53">
+        <v>12</v>
+      </c>
       <c r="Y53" s="1">
         <v>438.483</v>
       </c>
@@ -5569,7 +7216,9 @@
       <c r="C55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O55" s="2"/>
+      <c r="O55" t="s">
+        <v>34</v>
+      </c>
       <c r="R55" s="2" t="s">
         <v>13</v>
       </c>
@@ -5582,6 +7231,9 @@
       <c r="D56" t="s">
         <v>8</v>
       </c>
+      <c r="O56" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="R56" t="s">
         <v>1</v>
       </c>
@@ -5597,6 +7249,12 @@
       <c r="D57">
         <v>2</v>
       </c>
+      <c r="O57" t="s">
+        <v>1</v>
+      </c>
+      <c r="P57" t="s">
+        <v>0</v>
+      </c>
       <c r="R57">
         <v>722.11400000000003</v>
       </c>
@@ -5612,6 +7270,12 @@
       <c r="D58">
         <v>3</v>
       </c>
+      <c r="O58">
+        <v>93.042000000000002</v>
+      </c>
+      <c r="P58">
+        <v>1</v>
+      </c>
       <c r="R58">
         <v>605.98400000000004</v>
       </c>
@@ -5627,6 +7291,12 @@
       <c r="D59">
         <v>4</v>
       </c>
+      <c r="O59">
+        <v>46.486899999999999</v>
+      </c>
+      <c r="P59">
+        <v>2</v>
+      </c>
       <c r="R59">
         <v>588.18100000000004</v>
       </c>
@@ -5646,6 +7316,12 @@
       <c r="D60">
         <v>5</v>
       </c>
+      <c r="O60">
+        <v>31.541899999999998</v>
+      </c>
+      <c r="P60">
+        <v>3</v>
+      </c>
       <c r="R60">
         <v>447.09199999999998</v>
       </c>
@@ -5667,6 +7343,12 @@
       <c r="D61">
         <v>6</v>
       </c>
+      <c r="O61">
+        <v>23.744</v>
+      </c>
+      <c r="P61">
+        <v>4</v>
+      </c>
       <c r="R61">
         <v>396.25200000000001</v>
       </c>
@@ -5687,6 +7369,12 @@
       <c r="D62">
         <v>7</v>
       </c>
+      <c r="O62">
+        <v>19.869900000000001</v>
+      </c>
+      <c r="P62">
+        <v>5</v>
+      </c>
       <c r="R62">
         <v>235.53</v>
       </c>
@@ -5707,6 +7395,12 @@
       <c r="D63">
         <v>8</v>
       </c>
+      <c r="O63">
+        <v>19.519200000000001</v>
+      </c>
+      <c r="P63">
+        <v>6</v>
+      </c>
       <c r="R63">
         <v>328.86700000000002</v>
       </c>
@@ -5727,6 +7421,12 @@
       <c r="D64">
         <v>9</v>
       </c>
+      <c r="O64">
+        <v>19.569199999999999</v>
+      </c>
+      <c r="P64">
+        <v>7</v>
+      </c>
       <c r="R64">
         <v>195.29900000000001</v>
       </c>
@@ -5747,6 +7447,12 @@
       <c r="D65">
         <v>11</v>
       </c>
+      <c r="O65">
+        <v>19.6785</v>
+      </c>
+      <c r="P65">
+        <v>8</v>
+      </c>
       <c r="R65">
         <v>198.376</v>
       </c>
@@ -5767,6 +7473,12 @@
       <c r="D66">
         <v>12</v>
       </c>
+      <c r="O66">
+        <v>25.978999999999999</v>
+      </c>
+      <c r="P66">
+        <v>9</v>
+      </c>
       <c r="R66">
         <v>190.93</v>
       </c>
@@ -5781,6 +7493,12 @@
       </c>
     </row>
     <row r="67" spans="3:26">
+      <c r="O67">
+        <v>23.9206</v>
+      </c>
+      <c r="P67">
+        <v>10</v>
+      </c>
       <c r="R67">
         <v>174.899</v>
       </c>
@@ -5795,6 +7513,12 @@
       </c>
     </row>
     <row r="68" spans="3:26">
+      <c r="O68">
+        <v>23.7227</v>
+      </c>
+      <c r="P68">
+        <v>11</v>
+      </c>
       <c r="Y68">
         <v>220.53200000000001</v>
       </c>
@@ -5803,6 +7527,12 @@
       </c>
     </row>
     <row r="69" spans="3:26">
+      <c r="O69">
+        <v>23.723400000000002</v>
+      </c>
+      <c r="P69">
+        <v>12</v>
+      </c>
       <c r="Y69">
         <v>227.52099999999999</v>
       </c>
@@ -5857,7 +7587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="DM6" sqref="DM6:ED26"/>
     </sheetView>
   </sheetViews>
@@ -6876,15 +8606,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:R21"/>
+  <dimension ref="A8:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="8" spans="2:18">
+    <row r="8" spans="1:18">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -6894,6 +8624,9 @@
       <c r="H8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
       <c r="N8" s="2" t="s">
         <v>5</v>
       </c>
@@ -6901,7 +8634,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:18">
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -6920,6 +8656,12 @@
       <c r="I9" t="s">
         <v>0</v>
       </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
       <c r="N9" t="s">
         <v>1</v>
       </c>
@@ -6933,7 +8675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:18">
+    <row r="10" spans="1:18">
       <c r="B10">
         <v>419036</v>
       </c>
@@ -6952,6 +8694,12 @@
       <c r="I10">
         <v>1</v>
       </c>
+      <c r="L10">
+        <v>200000</v>
+      </c>
+      <c r="M10">
+        <v>400</v>
+      </c>
       <c r="N10">
         <v>50003</v>
       </c>
@@ -6965,7 +8713,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="2:18">
+    <row r="11" spans="1:18">
       <c r="B11">
         <v>211595</v>
       </c>
@@ -6984,6 +8732,12 @@
       <c r="I11">
         <v>2</v>
       </c>
+      <c r="L11" s="4">
+        <v>1060000</v>
+      </c>
+      <c r="M11">
+        <v>700</v>
+      </c>
       <c r="N11">
         <v>206030</v>
       </c>
@@ -6997,7 +8751,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="12" spans="2:18">
+    <row r="12" spans="1:18">
       <c r="B12">
         <v>146625</v>
       </c>
@@ -7016,6 +8770,12 @@
       <c r="I12">
         <v>3</v>
       </c>
+      <c r="L12" s="4">
+        <v>3170000</v>
+      </c>
+      <c r="M12">
+        <v>1000</v>
+      </c>
       <c r="N12">
         <v>522900</v>
       </c>
@@ -7029,7 +8789,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="2:18">
+    <row r="13" spans="1:18">
       <c r="B13">
         <v>109294</v>
       </c>
@@ -7048,6 +8808,12 @@
       <c r="I13">
         <v>4</v>
       </c>
+      <c r="L13" s="4">
+        <v>7060000</v>
+      </c>
+      <c r="M13">
+        <v>1300</v>
+      </c>
       <c r="N13" s="4">
         <v>1187200</v>
       </c>
@@ -7061,7 +8827,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="1:18">
       <c r="B14">
         <v>92766</v>
       </c>
@@ -7080,6 +8846,12 @@
       <c r="I14">
         <v>5</v>
       </c>
+      <c r="L14" s="4">
+        <v>13000000</v>
+      </c>
+      <c r="M14">
+        <v>1600</v>
+      </c>
       <c r="N14" s="4">
         <v>2544540</v>
       </c>
@@ -7093,7 +8865,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="1:18">
       <c r="B15">
         <v>81967</v>
       </c>
@@ -7112,6 +8884,12 @@
       <c r="I15">
         <v>6</v>
       </c>
+      <c r="L15" s="4">
+        <v>22830000</v>
+      </c>
+      <c r="M15">
+        <v>1900</v>
+      </c>
       <c r="N15" s="4">
         <v>4725060</v>
       </c>
@@ -7125,7 +8903,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="1:18">
       <c r="B16">
         <v>73487</v>
       </c>
@@ -7143,6 +8921,12 @@
       </c>
       <c r="I16">
         <v>7</v>
+      </c>
+      <c r="L16" s="4">
+        <v>36530000</v>
+      </c>
+      <c r="M16">
+        <v>2200</v>
       </c>
       <c r="N16" s="4">
         <v>8252550</v>
@@ -7176,6 +8960,12 @@
       <c r="I17">
         <v>8</v>
       </c>
+      <c r="L17" s="4">
+        <v>51410000</v>
+      </c>
+      <c r="M17">
+        <v>2500</v>
+      </c>
       <c r="N17" s="4">
         <v>11353800</v>
       </c>
@@ -7208,6 +8998,12 @@
       <c r="I18">
         <v>9</v>
       </c>
+      <c r="L18" s="4">
+        <v>85110000</v>
+      </c>
+      <c r="M18">
+        <v>2800</v>
+      </c>
       <c r="N18" s="4">
         <v>15994600</v>
       </c>
@@ -7240,6 +9036,12 @@
       <c r="I19">
         <v>10</v>
       </c>
+      <c r="L19" s="4">
+        <v>97330000</v>
+      </c>
+      <c r="M19">
+        <v>3100</v>
+      </c>
       <c r="N19" s="4">
         <v>21513200</v>
       </c>
@@ -7272,6 +9074,12 @@
       <c r="I20">
         <v>11</v>
       </c>
+      <c r="L20" s="4">
+        <v>144820000</v>
+      </c>
+      <c r="M20">
+        <v>3400</v>
+      </c>
       <c r="N20" s="4">
         <v>28267900</v>
       </c>
@@ -7303,6 +9111,12 @@
       </c>
       <c r="I21">
         <v>12</v>
+      </c>
+      <c r="L21" s="4">
+        <v>164520000</v>
+      </c>
+      <c r="M21">
+        <v>3700</v>
       </c>
       <c r="N21" s="4">
         <v>36457800</v>
@@ -7327,4 +9141,405 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="18">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="18">
+      <c r="A3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" ht="18">
+      <c r="A5" s="6">
+        <v>93.042000000000002</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1329.52</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5">
+        <f>B5/A5</f>
+        <v>14.289460673674254</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5">
+        <f>LOG10(3000)/LOG10(2)</f>
+        <v>11.550746785383243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="6">
+        <v>46.486899999999999</v>
+      </c>
+      <c r="B6" s="6">
+        <v>731.25199999999995</v>
+      </c>
+      <c r="C6" s="6">
+        <v>722.11400000000003</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f>B6/A6</f>
+        <v>15.730281003895721</v>
+      </c>
+      <c r="F6">
+        <f>C6/A6</f>
+        <v>15.533709496653897</v>
+      </c>
+      <c r="G6">
+        <f>E6/(LOG10(3000)/LOG10(2))</f>
+        <v>1.3618410390401268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18">
+      <c r="A7" s="6">
+        <v>31.541899999999998</v>
+      </c>
+      <c r="B7" s="6">
+        <v>576.30200000000002</v>
+      </c>
+      <c r="C7" s="6">
+        <v>605.98400000000004</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <f>B7/A7</f>
+        <v>18.270998259458057</v>
+      </c>
+      <c r="F7">
+        <f>C7/A7</f>
+        <v>19.212032249166985</v>
+      </c>
+      <c r="G7">
+        <f>E7/(LOG10(3000)/LOG10(2))</f>
+        <v>1.5818023370210901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18">
+      <c r="A8" s="6">
+        <v>23.744</v>
+      </c>
+      <c r="B8" s="6">
+        <v>449.05399999999997</v>
+      </c>
+      <c r="C8" s="6">
+        <v>588.18100000000004</v>
+      </c>
+      <c r="D8" s="6">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f>B8/A8</f>
+        <v>18.912314690026953</v>
+      </c>
+      <c r="F8">
+        <f>C8/A8</f>
+        <v>24.771773921832885</v>
+      </c>
+      <c r="G8">
+        <f>E8/(LOG10(3000)/LOG10(2))</f>
+        <v>1.6373239792564165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18">
+      <c r="A9" s="6">
+        <v>19.869900000000001</v>
+      </c>
+      <c r="B9" s="6">
+        <v>593.745</v>
+      </c>
+      <c r="C9" s="6">
+        <v>447.09199999999998</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>B9/A9</f>
+        <v>29.881630003170624</v>
+      </c>
+      <c r="F9">
+        <f>C9/A9</f>
+        <v>22.500968802057383</v>
+      </c>
+      <c r="G9">
+        <f>E9/(LOG10(3000)/LOG10(2))</f>
+        <v>2.586986846684578</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18">
+      <c r="A10" s="6">
+        <v>19.519200000000001</v>
+      </c>
+      <c r="B10" s="6">
+        <v>550.83799999999997</v>
+      </c>
+      <c r="C10" s="6">
+        <v>396.25200000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <f>B10/A10</f>
+        <v>28.220316406410095</v>
+      </c>
+      <c r="F10">
+        <f>C10/A10</f>
+        <v>20.300627074880119</v>
+      </c>
+      <c r="G10">
+        <f>E10/(LOG10(3000)/LOG10(2))</f>
+        <v>2.443159471050059</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18">
+      <c r="A11" s="6">
+        <v>19.569199999999999</v>
+      </c>
+      <c r="B11" s="6">
+        <v>510.23</v>
+      </c>
+      <c r="C11" s="6">
+        <v>235.53</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <f>B11/A11</f>
+        <v>26.073114894834742</v>
+      </c>
+      <c r="F11">
+        <f>C11/A11</f>
+        <v>12.035750056210782</v>
+      </c>
+      <c r="G11">
+        <f>E11/(LOG10(3000)/LOG10(2))</f>
+        <v>2.2572665975007484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18">
+      <c r="A12" s="6">
+        <v>19.6785</v>
+      </c>
+      <c r="B12" s="6">
+        <v>434.15300000000002</v>
+      </c>
+      <c r="C12" s="6">
+        <v>328.86700000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <f>B12/A12</f>
+        <v>22.062301496557158</v>
+      </c>
+      <c r="F12">
+        <f>C12/A12</f>
+        <v>16.711995324846914</v>
+      </c>
+      <c r="G12">
+        <f>E12/(LOG10(3000)/LOG10(2))</f>
+        <v>1.9100324772486259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18">
+      <c r="A13" s="6">
+        <v>25.978999999999999</v>
+      </c>
+      <c r="B13" s="6">
+        <v>424.99200000000002</v>
+      </c>
+      <c r="C13" s="6">
+        <v>195.29900000000001</v>
+      </c>
+      <c r="D13" s="6">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <f>B13/A13</f>
+        <v>16.35905924015551</v>
+      </c>
+      <c r="F13">
+        <f>C13/A13</f>
+        <v>7.5175718849840258</v>
+      </c>
+      <c r="G13">
+        <f>E13/(LOG10(3000)/LOG10(2))</f>
+        <v>1.4162771935107166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18">
+      <c r="A14" s="6">
+        <v>23.9206</v>
+      </c>
+      <c r="B14" s="6">
+        <v>385.13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>198.376</v>
+      </c>
+      <c r="D14" s="6">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <f>B14/A14</f>
+        <v>16.100348653461868</v>
+      </c>
+      <c r="F14">
+        <f>C14/A14</f>
+        <v>8.2931030158106402</v>
+      </c>
+      <c r="G14">
+        <f>E14/(LOG10(3000)/LOG10(2))</f>
+        <v>1.3938794566803132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18">
+      <c r="A15" s="6">
+        <v>23.7227</v>
+      </c>
+      <c r="B15" s="6">
+        <v>373.77300000000002</v>
+      </c>
+      <c r="C15" s="6">
+        <v>190.93</v>
+      </c>
+      <c r="D15" s="6">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <f>B15/A15</f>
+        <v>15.755921543500531</v>
+      </c>
+      <c r="F15">
+        <f>C15/A15</f>
+        <v>8.0484093294608119</v>
+      </c>
+      <c r="G15">
+        <f>E15/(LOG10(3000)/LOG10(2))</f>
+        <v>1.364060855652959</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18">
+      <c r="A16" s="6">
+        <v>23.723400000000002</v>
+      </c>
+      <c r="B16" s="6">
+        <v>151.33000000000001</v>
+      </c>
+      <c r="C16" s="6">
+        <v>174.899</v>
+      </c>
+      <c r="D16" s="6">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <f>B16/A16</f>
+        <v>6.378933879629396</v>
+      </c>
+      <c r="F16">
+        <f>C16/A16</f>
+        <v>7.3724255376548049</v>
+      </c>
+      <c r="G16">
+        <f>E16/(LOG10(3000)/LOG10(2))</f>
+        <v>0.55225294071042597</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added flops of square sum to results excel
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="0" windowWidth="14800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>Threads</t>
   </si>
@@ -227,6 +227,12 @@
   <si>
     <t>node</t>
   </si>
+  <si>
+    <t>FW Serial</t>
+  </si>
+  <si>
+    <t>Square sum serial</t>
+  </si>
 </sst>
 </file>
 
@@ -361,8 +367,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="599">
+  <cellStyleXfs count="603">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1017,7 +1027,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="599">
+  <cellStyles count="603">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1317,6 +1327,8 @@
     <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1616,6 +1628,8 @@
     <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1955,11 +1969,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116786472"/>
-        <c:axId val="2114685480"/>
+        <c:axId val="2119110072"/>
+        <c:axId val="2119100920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116786472"/>
+        <c:axId val="2119110072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.0"/>
@@ -1990,13 +2004,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114685480"/>
+        <c:crossAx val="2119100920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2114685480"/>
+        <c:axId val="2119100920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -2027,7 +2041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116786472"/>
+        <c:crossAx val="2119110072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2151,11 +2165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2114254696"/>
-        <c:axId val="2110251832"/>
+        <c:axId val="2128315832"/>
+        <c:axId val="2128321576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2114254696"/>
+        <c:axId val="2128315832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2188,7 +2202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110251832"/>
+        <c:crossAx val="2128321576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2196,7 +2210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110251832"/>
+        <c:axId val="2128321576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114254696"/>
+        <c:crossAx val="2128315832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2608,11 +2622,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108105688"/>
-        <c:axId val="2108111352"/>
+        <c:axId val="2128223176"/>
+        <c:axId val="2127756504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108105688"/>
+        <c:axId val="2128223176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2646,7 +2660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108111352"/>
+        <c:crossAx val="2127756504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2654,7 +2668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108111352"/>
+        <c:axId val="2127756504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,7 +2703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108105688"/>
+        <c:crossAx val="2128223176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2775,521 +2789,6 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> OMP Time Performance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>500 Nodes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$C$10:$C$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$A$10:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>8.710930383079816</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.725161726676421</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.195987298028508</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.772070392176643</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.535524229773216</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.35697129097458</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.19941715171615</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.141473664529821</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.952193763565091</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.777261891564584</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.77135740899056</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.723176267627523</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$E$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1000 Nodes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$C$10:$C$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$D$10:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>11.89658595079915</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.76708368462604</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.21182747138189</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.709526722603483</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.384542021773617</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.180856480277841</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.123283374638841</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.992759934973804</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.9130434748723</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.985955754607507</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.897601961767126</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.531032442069381</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$H$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3000 Nodes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$C$10:$C$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$G$10:$G$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>16.50559448838841</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.50453660184117</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.94498194640004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.5352753766208</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.2782969914492</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.25260630439266</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14.25629715852777</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.26433263452352</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.66505827827954</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.54596595663431</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.5339805991691</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14.53402316901271</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2109984376"/>
-        <c:axId val="2110183736"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2109984376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>#</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> of Threads</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110183736"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2110183736"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Time Spent on Computation</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>LOG2(ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109984376"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.806410072028668"/>
-          <c:y val="0.0289878361478107"/>
-          <c:w val="0.171635685950215"/>
-          <c:h val="0.137963655164222"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>FW</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
               <a:t> OMP vs SS OMP vs SS MPI</a:t>
             </a:r>
           </a:p>
@@ -3627,11 +3126,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109953192"/>
-        <c:axId val="2100918360"/>
+        <c:axId val="2127841576"/>
+        <c:axId val="2127847192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109953192"/>
+        <c:axId val="2127841576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3664,7 +3163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100918360"/>
+        <c:crossAx val="2127847192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3672,7 +3171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100918360"/>
+        <c:axId val="2127847192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3702,7 +3201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109953192"/>
+        <c:crossAx val="2127841576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3744,7 +3243,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4110,11 +3609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2114953944"/>
-        <c:axId val="2104827832"/>
+        <c:axId val="2127885096"/>
+        <c:axId val="2128074552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2114953944"/>
+        <c:axId val="2127885096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4143,7 +3642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104827832"/>
+        <c:crossAx val="2128074552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4151,7 +3650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104827832"/>
+        <c:axId val="2128074552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4186,7 +3685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114953944"/>
+        <c:crossAx val="2127885096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4228,7 +3727,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4604,11 +4103,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108148200"/>
-        <c:axId val="2108153720"/>
+        <c:axId val="2128237512"/>
+        <c:axId val="2127953352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108148200"/>
+        <c:axId val="2128237512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4637,7 +4136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108153720"/>
+        <c:crossAx val="2127953352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4645,7 +4144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108153720"/>
+        <c:axId val="2127953352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4675,7 +4174,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108148200"/>
+        <c:crossAx val="2128237512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4726,7 +4225,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4995,11 +4494,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106879784"/>
-        <c:axId val="2106885272"/>
+        <c:axId val="2111937192"/>
+        <c:axId val="2111990424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106879784"/>
+        <c:axId val="2111937192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5027,7 +4526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106885272"/>
+        <c:crossAx val="2111990424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5035,7 +4534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106885272"/>
+        <c:axId val="2111990424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5064,7 +4563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106879784"/>
+        <c:crossAx val="2111937192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5079,6 +4578,464 @@
           <c:y val="0.166815617767129"/>
           <c:w val="0.22703220770873"/>
           <c:h val="0.112352528650942"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Logarithmic Speedup Plot (3000 Nodes)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>FW OMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet4!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$L$6:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.001057886547243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.560612541988378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.970319111767614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.227297496939211</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.252988183995755</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.249297329860641</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.241261853864897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.840536210108874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.959628531754107</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.971613889219323</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.971571319375702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SS OMP</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet4!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$M$6:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.974414651458994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.630871012514402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.270934929562347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.673889445317318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.565674074425641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.455193713641876</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.222249538954344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.191481670430605</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.04939149340943</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.006208343860805</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.701744005069644</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>SS MPI</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet4!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$N$6:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.956272599132825</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.703325688285586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.66030616767476</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.264617717427528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.090464203023595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.339956816989293</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.821550234948626</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.069730548182805</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.092283481655315</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.03708979099445</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.910568026599183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2121466632"/>
+        <c:axId val="2121455944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2121466632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t># of Threads/Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121455944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121455944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>LOG2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (Speedup)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121466632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.800511299723898"/>
+          <c:y val="0.771378371092043"/>
+          <c:w val="0.15310651103677"/>
+          <c:h val="0.176487649787578"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -5140,464 +5097,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Logarithmic Speedup Plot (3000 Nodes)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>FW OMP</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet4!$D$6:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet4!$L$6:$L$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.001057886547243</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.560612541988378</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.970319111767614</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.227297496939211</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.252988183995755</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.249297329860641</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.241261853864897</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.840536210108874</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.959628531754107</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.971613889219323</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.971571319375702</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>SS OMP</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet4!$D$6:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet4!$M$6:$M$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>-2.974414651458994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.630871012514402</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.270934929562347</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2.673889445317318</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2.565674074425641</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2.455193713641876</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2.222249538954344</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2.191481670430605</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-2.04939149340943</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-2.006208343860805</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.701744005069644</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>SS MPI</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet4!$D$6:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet4!$N$6:$N$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>-2.956272599132825</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.703325688285586</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.66030616767476</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2.264617717427528</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2.090464203023595</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1.339956816989293</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.821550234948626</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.069730548182805</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.092283481655315</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.03708979099445</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.910568026599183</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2117017784"/>
-        <c:axId val="2116622504"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2117017784"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t># of Threads/Processes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116622504"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2116622504"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>LOG2</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> (Speedup)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117017784"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.800511299723898"/>
-          <c:y val="0.771378371092043"/>
-          <c:w val="0.15310651103677"/>
-          <c:h val="0.176487649787578"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Speedup</a:t>
             </a:r>
             <a:r>
@@ -5911,11 +5410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116766728"/>
-        <c:axId val="2100393752"/>
+        <c:axId val="2101791432"/>
+        <c:axId val="2122236984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116766728"/>
+        <c:axId val="2101791432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5943,7 +5442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100393752"/>
+        <c:crossAx val="2122236984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5951,7 +5450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100393752"/>
+        <c:axId val="2122236984"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5981,7 +5480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116766728"/>
+        <c:crossAx val="2101791432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6393,11 +5892,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116743416"/>
-        <c:axId val="2116759432"/>
+        <c:axId val="2118979000"/>
+        <c:axId val="2118984456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116743416"/>
+        <c:axId val="2118979000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6426,12 +5925,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116759432"/>
+        <c:crossAx val="2118984456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116759432"/>
+        <c:axId val="2118984456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6466,7 +5965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116743416"/>
+        <c:crossAx val="2118979000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6827,11 +6326,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117027192"/>
-        <c:axId val="2116838936"/>
+        <c:axId val="2118951224"/>
+        <c:axId val="2118910888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117027192"/>
+        <c:axId val="2118951224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6865,7 +6364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116838936"/>
+        <c:crossAx val="2118910888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6873,7 +6372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116838936"/>
+        <c:axId val="2118910888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6908,7 +6407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117027192"/>
+        <c:crossAx val="2118951224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7104,11 +6603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122182584"/>
-        <c:axId val="2101909768"/>
+        <c:axId val="2118875544"/>
+        <c:axId val="2118881016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122182584"/>
+        <c:axId val="2118875544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7137,12 +6636,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101909768"/>
+        <c:crossAx val="2118881016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2101909768"/>
+        <c:axId val="2118881016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7172,7 +6671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122182584"/>
+        <c:crossAx val="2118875544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7779,11 +7278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2114991016"/>
-        <c:axId val="2114994168"/>
+        <c:axId val="2127747736"/>
+        <c:axId val="2115522728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2114991016"/>
+        <c:axId val="2127747736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14.0"/>
@@ -7814,12 +7313,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114994168"/>
+        <c:crossAx val="2115522728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2114994168"/>
+        <c:axId val="2115522728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -7850,7 +7349,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114991016"/>
+        <c:crossAx val="2127747736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8327,11 +7826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2106993160"/>
-        <c:axId val="2097418120"/>
+        <c:axId val="2127685896"/>
+        <c:axId val="2127615352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2106993160"/>
+        <c:axId val="2127685896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8365,12 +7864,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097418120"/>
+        <c:crossAx val="2127615352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097418120"/>
+        <c:axId val="2127615352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8400,7 +7899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106993160"/>
+        <c:crossAx val="2127685896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8436,10 +7935,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -8450,39 +7945,42 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Floyd Warshall</c:v>
+            <c:v>Floyd Warshall </c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$74:$D$82</c:f>
+              <c:f>Sheet2!$D$74:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>700.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1000.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1300.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1600.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1900.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2200.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2500.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2800.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3100.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -8490,36 +7988,125 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$74:$C$82</c:f>
+              <c:f>Sheet2!$C$74:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1280.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1276.28</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>1161.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1124.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1137.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1143.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1002.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1159.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1170.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Square Sum</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$O$75:$O$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>400.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1161.1</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1124.5</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1137.38</c:v>
+                  <c:v>1300.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1143.64</c:v>
+                  <c:v>1600.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1002.75</c:v>
+                  <c:v>1900.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1159.02</c:v>
+                  <c:v>2200.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1170.62</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1142.46</c:v>
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$N$75:$N$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1280.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>724.011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>166.147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137.312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>158.952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159.721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>408.335</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146.391</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>141.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8534,11 +8121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115548952"/>
-        <c:axId val="2116817672"/>
+        <c:axId val="2127640936"/>
+        <c:axId val="2127646344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115548952"/>
+        <c:axId val="2127640936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8567,12 +8154,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116817672"/>
+        <c:crossAx val="2127646344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116817672"/>
+        <c:axId val="2127646344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8602,7 +8189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115548952"/>
+        <c:crossAx val="2127640936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8731,11 +8318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100910424"/>
-        <c:axId val="2097532168"/>
+        <c:axId val="2127695608"/>
+        <c:axId val="2127701320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100910424"/>
+        <c:axId val="2127695608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8768,7 +8355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097532168"/>
+        <c:crossAx val="2127701320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8776,7 +8363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097532168"/>
+        <c:axId val="2127701320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8811,7 +8398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100910424"/>
+        <c:crossAx val="2127695608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8935,11 +8522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108504136"/>
-        <c:axId val="2108509560"/>
+        <c:axId val="2127944984"/>
+        <c:axId val="2128287736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108504136"/>
+        <c:axId val="2127944984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8967,7 +8554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108509560"/>
+        <c:crossAx val="2128287736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8975,7 +8562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108509560"/>
+        <c:axId val="2128287736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9010,7 +8597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108504136"/>
+        <c:crossAx val="2127944984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9217,13 +8804,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>558800</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
@@ -9371,38 +8958,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -9425,7 +8980,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9455,7 +9010,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9463,16 +9018,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9485,7 +9040,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9913,7 +9468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:AD101"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="E16" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
@@ -11454,10 +11009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W82"/>
+  <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7:S10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="N84" sqref="N84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12850,94 +12405,178 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="3:7">
+    <row r="65" spans="3:15">
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="3:7">
+    <row r="66" spans="3:15">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="3:7">
+    <row r="67" spans="3:15">
       <c r="G67" s="1"/>
     </row>
-    <row r="73" spans="3:7">
+    <row r="72" spans="3:15">
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="3:15">
       <c r="C73" t="s">
         <v>66</v>
       </c>
       <c r="D73" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="74" spans="3:7">
+      <c r="N73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="3:15">
       <c r="C74">
+        <v>1280</v>
+      </c>
+      <c r="D74">
+        <v>400</v>
+      </c>
+      <c r="N74" t="s">
+        <v>66</v>
+      </c>
+      <c r="O74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="3:15">
+      <c r="C75">
         <v>1276.28</v>
       </c>
-      <c r="D74">
+      <c r="D75">
         <v>700</v>
       </c>
-    </row>
-    <row r="75" spans="3:7">
-      <c r="C75">
+      <c r="N75">
+        <v>1280</v>
+      </c>
+      <c r="O75">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="3:15">
+      <c r="C76">
         <v>1161.0999999999999</v>
       </c>
-      <c r="D75">
+      <c r="D76">
         <v>1000</v>
       </c>
-    </row>
-    <row r="76" spans="3:7">
-      <c r="C76">
+      <c r="N76">
+        <v>724.01099999999997</v>
+      </c>
+      <c r="O76">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="77" spans="3:15">
+      <c r="C77">
         <v>1124.5</v>
       </c>
-      <c r="D76">
+      <c r="D77">
         <v>1300</v>
       </c>
-    </row>
-    <row r="77" spans="3:7">
-      <c r="C77">
+      <c r="N77">
+        <v>166.14699999999999</v>
+      </c>
+      <c r="O77">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="78" spans="3:15">
+      <c r="C78">
         <v>1137.3800000000001</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>1600</v>
       </c>
-    </row>
-    <row r="78" spans="3:7">
-      <c r="C78">
+      <c r="N78">
+        <v>137.31200000000001</v>
+      </c>
+      <c r="O78">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="79" spans="3:15">
+      <c r="C79">
         <v>1143.6400000000001</v>
       </c>
-      <c r="D78">
+      <c r="D79">
         <v>1900</v>
       </c>
-    </row>
-    <row r="79" spans="3:7">
-      <c r="C79">
+      <c r="N79">
+        <v>158.952</v>
+      </c>
+      <c r="O79">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="80" spans="3:15">
+      <c r="C80">
         <v>1002.75</v>
       </c>
-      <c r="D79">
+      <c r="D80">
         <v>2200</v>
       </c>
-    </row>
-    <row r="80" spans="3:7">
-      <c r="C80">
+      <c r="N80">
+        <v>159.721</v>
+      </c>
+      <c r="O80">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="81" spans="3:15">
+      <c r="C81">
         <v>1159.02</v>
       </c>
-      <c r="D80">
+      <c r="D81">
         <v>2500</v>
       </c>
-    </row>
-    <row r="81" spans="3:4">
-      <c r="C81">
+      <c r="N81">
+        <v>408.33499999999998</v>
+      </c>
+      <c r="O81">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="82" spans="3:15">
+      <c r="C82">
         <v>1170.6199999999999</v>
       </c>
-      <c r="D81">
+      <c r="D82">
         <v>2800</v>
       </c>
-    </row>
-    <row r="82" spans="3:4">
-      <c r="C82">
+      <c r="N82">
+        <v>128.88900000000001</v>
+      </c>
+      <c r="O82">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="83" spans="3:15">
+      <c r="C83">
         <v>1142.46</v>
       </c>
-      <c r="D82">
+      <c r="D83">
+        <v>3100</v>
+      </c>
+      <c r="N83">
+        <v>146.39099999999999</v>
+      </c>
+      <c r="O83">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="84" spans="3:15">
+      <c r="N84">
+        <v>141.88</v>
+      </c>
+      <c r="O84">
         <v>3100</v>
       </c>
     </row>
@@ -12950,6 +12589,7 @@
     <mergeCell ref="V37:W37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -12963,7 +12603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A99" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>

</xml_diff>